<commit_message>
Menu Resultado Funcionando Corretamente
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -825,9 +825,197 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B10">
+        <v>1578424633</v>
+      </c>
+      <c r="C10" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>11</v>
+      </c>
+      <c r="N10">
+        <v>38</v>
+      </c>
+      <c r="O10" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B11">
+        <v>1578424633</v>
+      </c>
+      <c r="C11" t="str">
+        <v>11900009999</v>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B12">
+        <v>1578424633</v>
+      </c>
+      <c r="C12" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>9</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B13">
+        <v>1578424633</v>
+      </c>
+      <c r="C13" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D13" t="str">
+        <v/>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <v>9</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="O13" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Faltando apenas parte de pagamento
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1013,9 +1013,103 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B14">
+        <v>1578424633</v>
+      </c>
+      <c r="C14" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="K14">
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <v>9</v>
+      </c>
+      <c r="N14">
+        <v>10</v>
+      </c>
+      <c r="O14" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B15">
+        <v>1578424633</v>
+      </c>
+      <c r="C15" t="str">
+        <v>119988776655</v>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>11</v>
+      </c>
+      <c r="J15">
+        <v>12</v>
+      </c>
+      <c r="K15">
+        <v>16</v>
+      </c>
+      <c r="L15">
+        <v>17</v>
+      </c>
+      <c r="M15">
+        <v>21</v>
+      </c>
+      <c r="N15">
+        <v>22</v>
+      </c>
+      <c r="O15" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ESTÉTICA OK,FALTANDO APENAS QUANDO O ÚSUARIO DIGITAR PARA IR PARA OS MENUS
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -836,7 +836,7 @@
         <v>11966548087</v>
       </c>
       <c r="D10" t="str">
-        <v/>
+        <v>76941312538</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -883,7 +883,7 @@
         <v>11900009999</v>
       </c>
       <c r="D11" t="str">
-        <v/>
+        <v>76705028247</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -930,7 +930,7 @@
         <v>11966548087</v>
       </c>
       <c r="D12" t="str">
-        <v/>
+        <v>76946688512</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -977,7 +977,7 @@
         <v>11966548087</v>
       </c>
       <c r="D13" t="str">
-        <v/>
+        <v>76946729412</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1024,7 +1024,7 @@
         <v>11966548087</v>
       </c>
       <c r="D14" t="str">
-        <v/>
+        <v>76946761994</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1071,7 +1071,7 @@
         <v>119988776655</v>
       </c>
       <c r="D15" t="str">
-        <v/>
+        <v>76947984334</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1107,9 +1107,620 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B16">
+        <v>1578424633</v>
+      </c>
+      <c r="C16" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D16" t="str">
+        <v>76947869106</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>7</v>
+      </c>
+      <c r="L16">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>9</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+      <c r="O16" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B17">
+        <v>1578424633</v>
+      </c>
+      <c r="C17" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D17" t="str">
+        <v>76947967362</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>9</v>
+      </c>
+      <c r="N17">
+        <v>10</v>
+      </c>
+      <c r="O17" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B18">
+        <v>1578424633</v>
+      </c>
+      <c r="C18" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D18" t="str">
+        <v>76948023750</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>7</v>
+      </c>
+      <c r="L18">
+        <v>8</v>
+      </c>
+      <c r="M18">
+        <v>9</v>
+      </c>
+      <c r="N18">
+        <v>10</v>
+      </c>
+      <c r="O18" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B19">
+        <v>1578424633</v>
+      </c>
+      <c r="C19" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D19" t="str">
+        <v>76707382593</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>6</v>
+      </c>
+      <c r="K19">
+        <v>7</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B20">
+        <v>1578424633</v>
+      </c>
+      <c r="C20" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D20" t="str">
+        <v>76707312891</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>7</v>
+      </c>
+      <c r="L20">
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <v>9</v>
+      </c>
+      <c r="N20">
+        <v>10</v>
+      </c>
+      <c r="O20" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B21">
+        <v>1578424633</v>
+      </c>
+      <c r="C21" t="str">
+        <v>11966548088</v>
+      </c>
+      <c r="D21" t="str">
+        <v>76707460717</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>6</v>
+      </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <v>9</v>
+      </c>
+      <c r="N21">
+        <v>10</v>
+      </c>
+      <c r="O21" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B22">
+        <v>1578424633</v>
+      </c>
+      <c r="C22" t="str">
+        <v>11977665544</v>
+      </c>
+      <c r="D22" t="str">
+        <v>76950373414</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>6</v>
+      </c>
+      <c r="K22">
+        <v>7</v>
+      </c>
+      <c r="L22">
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <v>9</v>
+      </c>
+      <c r="N22">
+        <v>10</v>
+      </c>
+      <c r="O22" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B23">
+        <v>1578424633</v>
+      </c>
+      <c r="C23" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D23" t="str">
+        <v/>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>6</v>
+      </c>
+      <c r="K23">
+        <v>7</v>
+      </c>
+      <c r="L23">
+        <v>8</v>
+      </c>
+      <c r="M23">
+        <v>9</v>
+      </c>
+      <c r="N23">
+        <v>10</v>
+      </c>
+      <c r="O23" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B24">
+        <v>1578424633</v>
+      </c>
+      <c r="C24" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D24" t="str">
+        <v/>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <v>7</v>
+      </c>
+      <c r="L24">
+        <v>8</v>
+      </c>
+      <c r="M24">
+        <v>9</v>
+      </c>
+      <c r="N24">
+        <v>10</v>
+      </c>
+      <c r="O24" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B25">
+        <v>1578424633</v>
+      </c>
+      <c r="C25" t="str">
+        <v>11977665544</v>
+      </c>
+      <c r="D25" t="str">
+        <v/>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="J25">
+        <v>6</v>
+      </c>
+      <c r="K25">
+        <v>7</v>
+      </c>
+      <c r="L25">
+        <v>8</v>
+      </c>
+      <c r="M25">
+        <v>9</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+      <c r="O25" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B26">
+        <v>1578424633</v>
+      </c>
+      <c r="C26" t="str">
+        <v>11977665544</v>
+      </c>
+      <c r="D26" t="str">
+        <v/>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>7</v>
+      </c>
+      <c r="L26">
+        <v>8</v>
+      </c>
+      <c r="M26">
+        <v>9</v>
+      </c>
+      <c r="N26">
+        <v>10</v>
+      </c>
+      <c r="O26" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B27">
+        <v>1578424633</v>
+      </c>
+      <c r="C27" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D27" t="str">
+        <v/>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+      <c r="K27">
+        <v>7</v>
+      </c>
+      <c r="L27">
+        <v>8</v>
+      </c>
+      <c r="M27">
+        <v>9</v>
+      </c>
+      <c r="N27">
+        <v>10</v>
+      </c>
+      <c r="O27" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B28">
+        <v>1578424633</v>
+      </c>
+      <c r="C28" t="str">
+        <v>11977665544</v>
+      </c>
+      <c r="D28" t="str">
+        <v/>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>6</v>
+      </c>
+      <c r="K28">
+        <v>7</v>
+      </c>
+      <c r="L28">
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <v>9</v>
+      </c>
+      <c r="N28">
+        <v>10</v>
+      </c>
+      <c r="O28" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O28"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ESTÉTICA E BOTÕES OK
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1447,7 +1447,7 @@
         <v>11966548087</v>
       </c>
       <c r="D23" t="str">
-        <v/>
+        <v>76955304908</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1718,9 +1718,56 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B29">
+        <v>1578424633</v>
+      </c>
+      <c r="C29" t="str">
+        <v>11966554433</v>
+      </c>
+      <c r="D29" t="str">
+        <v/>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
+      </c>
+      <c r="K29">
+        <v>7</v>
+      </c>
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="M29">
+        <v>9</v>
+      </c>
+      <c r="N29">
+        <v>10</v>
+      </c>
+      <c r="O29" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O28"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TIRANDO AS MENSAGENS ANTERIORES ANTES DE GERAR O QR CODE
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1494,7 +1494,7 @@
         <v>11988776655</v>
       </c>
       <c r="D24" t="str">
-        <v/>
+        <v>76956334770</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1541,7 +1541,7 @@
         <v>11977665544</v>
       </c>
       <c r="D25" t="str">
-        <v/>
+        <v>76956534748</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1588,7 +1588,7 @@
         <v>11977665544</v>
       </c>
       <c r="D26" t="str">
-        <v/>
+        <v>76956509396</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1765,9 +1765,150 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B30">
+        <v>1578424633</v>
+      </c>
+      <c r="C30" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>6</v>
+      </c>
+      <c r="K30">
+        <v>7</v>
+      </c>
+      <c r="L30">
+        <v>8</v>
+      </c>
+      <c r="M30">
+        <v>9</v>
+      </c>
+      <c r="N30">
+        <v>10</v>
+      </c>
+      <c r="O30" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B31">
+        <v>1578424633</v>
+      </c>
+      <c r="C31" t="str">
+        <v>11977665544</v>
+      </c>
+      <c r="D31" t="str">
+        <v/>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>6</v>
+      </c>
+      <c r="K31">
+        <v>7</v>
+      </c>
+      <c r="L31">
+        <v>8</v>
+      </c>
+      <c r="M31">
+        <v>9</v>
+      </c>
+      <c r="N31">
+        <v>10</v>
+      </c>
+      <c r="O31" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B32">
+        <v>1578424633</v>
+      </c>
+      <c r="C32" t="str">
+        <v>11887766554</v>
+      </c>
+      <c r="D32" t="str">
+        <v/>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>6</v>
+      </c>
+      <c r="K32">
+        <v>7</v>
+      </c>
+      <c r="L32">
+        <v>8</v>
+      </c>
+      <c r="M32">
+        <v>9</v>
+      </c>
+      <c r="N32">
+        <v>10</v>
+      </c>
+      <c r="O32" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O32"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionando a logo antes do QR CODE
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1635,7 +1635,7 @@
         <v>11988776655</v>
       </c>
       <c r="D27" t="str">
-        <v/>
+        <v>76958526368</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1906,9 +1906,56 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B33">
+        <v>1578424633</v>
+      </c>
+      <c r="C33" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D33" t="str">
+        <v/>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33">
+        <v>6</v>
+      </c>
+      <c r="K33">
+        <v>7</v>
+      </c>
+      <c r="L33">
+        <v>8</v>
+      </c>
+      <c r="M33">
+        <v>9</v>
+      </c>
+      <c r="N33">
+        <v>10</v>
+      </c>
+      <c r="O33" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O32"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alguns problemas de estética porém funcionando ainda
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1682,7 +1682,7 @@
         <v>11977665544</v>
       </c>
       <c r="D28" t="str">
-        <v/>
+        <v>76883386525</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1953,9 +1953,56 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B34">
+        <v>1578424633</v>
+      </c>
+      <c r="C34" t="str">
+        <v>11966554411</v>
+      </c>
+      <c r="D34" t="str">
+        <v/>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
+      <c r="K34">
+        <v>7</v>
+      </c>
+      <c r="L34">
+        <v>8</v>
+      </c>
+      <c r="M34">
+        <v>9</v>
+      </c>
+      <c r="N34">
+        <v>10</v>
+      </c>
+      <c r="O34" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O33"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O34"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alterações e Correções feitas, faltando estética de apagar Escolha 10 números
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1729,7 +1729,7 @@
         <v>11966554433</v>
       </c>
       <c r="D29" t="str">
-        <v/>
+        <v>76999025539</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1776,7 +1776,7 @@
         <v>11988776655</v>
       </c>
       <c r="D30" t="str">
-        <v/>
+        <v>77243067266</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1823,7 +1823,7 @@
         <v>11977665544</v>
       </c>
       <c r="D31" t="str">
-        <v/>
+        <v>77243137454</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1870,7 +1870,7 @@
         <v>11887766554</v>
       </c>
       <c r="D32" t="str">
-        <v/>
+        <v>77000631317</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1917,7 +1917,7 @@
         <v>11988776655</v>
       </c>
       <c r="D33" t="str">
-        <v/>
+        <v>77001090761</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1964,45 +1964,609 @@
         <v>11966554411</v>
       </c>
       <c r="D34" t="str">
+        <v>77001235025</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
+      <c r="K34">
+        <v>7</v>
+      </c>
+      <c r="L34">
+        <v>8</v>
+      </c>
+      <c r="M34">
+        <v>9</v>
+      </c>
+      <c r="N34">
+        <v>10</v>
+      </c>
+      <c r="O34" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B35">
+        <v>1578424633</v>
+      </c>
+      <c r="C35" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D35" t="str">
+        <v>77001321047</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>5</v>
+      </c>
+      <c r="J35">
+        <v>6</v>
+      </c>
+      <c r="K35">
+        <v>7</v>
+      </c>
+      <c r="L35">
+        <v>8</v>
+      </c>
+      <c r="M35">
+        <v>9</v>
+      </c>
+      <c r="N35">
+        <v>10</v>
+      </c>
+      <c r="O35" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B36">
+        <v>1578424633</v>
+      </c>
+      <c r="C36" t="str">
+        <v>11966554411</v>
+      </c>
+      <c r="D36" t="str">
+        <v>77243935384</v>
+      </c>
+      <c r="E36">
+        <v>18</v>
+      </c>
+      <c r="F36">
+        <v>29</v>
+      </c>
+      <c r="G36">
+        <v>31</v>
+      </c>
+      <c r="H36">
+        <v>32</v>
+      </c>
+      <c r="I36">
+        <v>34</v>
+      </c>
+      <c r="J36">
+        <v>44</v>
+      </c>
+      <c r="K36">
+        <v>45</v>
+      </c>
+      <c r="L36">
+        <v>47</v>
+      </c>
+      <c r="M36">
+        <v>48</v>
+      </c>
+      <c r="N36">
+        <v>50</v>
+      </c>
+      <c r="O36" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B37">
+        <v>1578424633</v>
+      </c>
+      <c r="C37" t="str">
+        <v>12965487563</v>
+      </c>
+      <c r="D37" t="str">
+        <v>77001321967</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>7</v>
+      </c>
+      <c r="K37">
+        <v>8</v>
+      </c>
+      <c r="L37">
+        <v>9</v>
+      </c>
+      <c r="M37">
+        <v>10</v>
+      </c>
+      <c r="N37">
+        <v>12</v>
+      </c>
+      <c r="O37" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B38">
+        <v>1578424633</v>
+      </c>
+      <c r="C38" t="str">
+        <v>11955448877</v>
+      </c>
+      <c r="D38" t="str">
+        <v>77244329042</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+      <c r="J38">
+        <v>6</v>
+      </c>
+      <c r="K38">
+        <v>7</v>
+      </c>
+      <c r="L38">
+        <v>8</v>
+      </c>
+      <c r="M38">
+        <v>9</v>
+      </c>
+      <c r="N38">
+        <v>10</v>
+      </c>
+      <c r="O38" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B39">
+        <v>1578424633</v>
+      </c>
+      <c r="C39" t="str">
+        <v>11966554422</v>
+      </c>
+      <c r="D39" t="str">
+        <v>77001940671</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <v>6</v>
+      </c>
+      <c r="K39">
+        <v>7</v>
+      </c>
+      <c r="L39">
+        <v>8</v>
+      </c>
+      <c r="M39">
+        <v>9</v>
+      </c>
+      <c r="N39">
+        <v>10</v>
+      </c>
+      <c r="O39" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B40">
+        <v>1578424633</v>
+      </c>
+      <c r="C40" t="str">
+        <v>11988775566</v>
+      </c>
+      <c r="D40" t="str">
+        <v>77244499150</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>6</v>
+      </c>
+      <c r="K40">
+        <v>7</v>
+      </c>
+      <c r="L40">
+        <v>8</v>
+      </c>
+      <c r="M40">
+        <v>9</v>
+      </c>
+      <c r="N40">
+        <v>10</v>
+      </c>
+      <c r="O40" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B41">
+        <v>1578424633</v>
+      </c>
+      <c r="C41" t="str">
+        <v>11966554400</v>
+      </c>
+      <c r="D41" t="str">
         <v/>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>2</v>
-      </c>
-      <c r="G34">
-        <v>3</v>
-      </c>
-      <c r="H34">
-        <v>4</v>
-      </c>
-      <c r="I34">
-        <v>5</v>
-      </c>
-      <c r="J34">
-        <v>6</v>
-      </c>
-      <c r="K34">
-        <v>7</v>
-      </c>
-      <c r="L34">
-        <v>8</v>
-      </c>
-      <c r="M34">
-        <v>9</v>
-      </c>
-      <c r="N34">
-        <v>10</v>
-      </c>
-      <c r="O34" t="str">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="J41">
+        <v>6</v>
+      </c>
+      <c r="K41">
+        <v>7</v>
+      </c>
+      <c r="L41">
+        <v>8</v>
+      </c>
+      <c r="M41">
+        <v>9</v>
+      </c>
+      <c r="N41">
+        <v>10</v>
+      </c>
+      <c r="O41" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B42">
+        <v>1578424633</v>
+      </c>
+      <c r="C42" t="str">
+        <v/>
+      </c>
+      <c r="D42" t="str">
+        <v/>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>5</v>
+      </c>
+      <c r="J42">
+        <v>6</v>
+      </c>
+      <c r="K42">
+        <v>7</v>
+      </c>
+      <c r="L42">
+        <v>8</v>
+      </c>
+      <c r="M42">
+        <v>9</v>
+      </c>
+      <c r="N42">
+        <v>10</v>
+      </c>
+      <c r="O42" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B43">
+        <v>1578424633</v>
+      </c>
+      <c r="C43" t="str">
+        <v>11966554422</v>
+      </c>
+      <c r="D43" t="str">
+        <v/>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>6</v>
+      </c>
+      <c r="K43">
+        <v>7</v>
+      </c>
+      <c r="L43">
+        <v>8</v>
+      </c>
+      <c r="M43">
+        <v>9</v>
+      </c>
+      <c r="N43">
+        <v>10</v>
+      </c>
+      <c r="O43" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B44">
+        <v>1578424633</v>
+      </c>
+      <c r="C44" t="str">
+        <v/>
+      </c>
+      <c r="D44" t="str">
+        <v/>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>6</v>
+      </c>
+      <c r="K44">
+        <v>7</v>
+      </c>
+      <c r="L44">
+        <v>8</v>
+      </c>
+      <c r="M44">
+        <v>9</v>
+      </c>
+      <c r="N44">
+        <v>10</v>
+      </c>
+      <c r="O44" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B45">
+        <v>1578424633</v>
+      </c>
+      <c r="C45" t="str">
+        <v>11988553322</v>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="I45">
+        <v>5</v>
+      </c>
+      <c r="J45">
+        <v>6</v>
+      </c>
+      <c r="K45">
+        <v>7</v>
+      </c>
+      <c r="L45">
+        <v>8</v>
+      </c>
+      <c r="M45">
+        <v>9</v>
+      </c>
+      <c r="N45">
+        <v>10</v>
+      </c>
+      <c r="O45" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B46">
+        <v>1578424633</v>
+      </c>
+      <c r="C46" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D46" t="str">
+        <v/>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>5</v>
+      </c>
+      <c r="J46">
+        <v>6</v>
+      </c>
+      <c r="K46">
+        <v>7</v>
+      </c>
+      <c r="L46">
+        <v>8</v>
+      </c>
+      <c r="M46">
+        <v>9</v>
+      </c>
+      <c r="N46">
+        <v>10</v>
+      </c>
+      <c r="O46" t="str">
         <v>Não</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O34"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O46"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Teclado sendo apagado com sucesso, e voltar do tevlado funcionando, faltando apenas o confirmar
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2293,7 +2293,7 @@
         <v>11966554400</v>
       </c>
       <c r="D41" t="str">
-        <v/>
+        <v>77280262910</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2340,7 +2340,7 @@
         <v/>
       </c>
       <c r="D42" t="str">
-        <v/>
+        <v>77282715892</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -2387,7 +2387,7 @@
         <v>11966554422</v>
       </c>
       <c r="D43" t="str">
-        <v/>
+        <v>77051216465</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -2434,7 +2434,7 @@
         <v/>
       </c>
       <c r="D44" t="str">
-        <v/>
+        <v>77298316438</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2481,7 +2481,7 @@
         <v>11988553322</v>
       </c>
       <c r="D45" t="str">
-        <v/>
+        <v>77055139631</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -2528,45 +2528,515 @@
         <v>11966548087</v>
       </c>
       <c r="D46" t="str">
+        <v>77298317798</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>5</v>
+      </c>
+      <c r="J46">
+        <v>6</v>
+      </c>
+      <c r="K46">
+        <v>7</v>
+      </c>
+      <c r="L46">
+        <v>8</v>
+      </c>
+      <c r="M46">
+        <v>9</v>
+      </c>
+      <c r="N46">
+        <v>10</v>
+      </c>
+      <c r="O46" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B47">
+        <v>1578424633</v>
+      </c>
+      <c r="C47" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D47" t="str">
+        <v>77299240172</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>3</v>
+      </c>
+      <c r="H47">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>5</v>
+      </c>
+      <c r="J47">
+        <v>6</v>
+      </c>
+      <c r="K47">
+        <v>7</v>
+      </c>
+      <c r="L47">
+        <v>8</v>
+      </c>
+      <c r="M47">
+        <v>9</v>
+      </c>
+      <c r="N47">
+        <v>10</v>
+      </c>
+      <c r="O47" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B48">
+        <v>1578424633</v>
+      </c>
+      <c r="C48" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D48" t="str">
+        <v>77056098875</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+      <c r="I48">
+        <v>5</v>
+      </c>
+      <c r="J48">
+        <v>6</v>
+      </c>
+      <c r="K48">
+        <v>7</v>
+      </c>
+      <c r="L48">
+        <v>8</v>
+      </c>
+      <c r="M48">
+        <v>9</v>
+      </c>
+      <c r="N48">
+        <v>10</v>
+      </c>
+      <c r="O48" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B49">
+        <v>1578424633</v>
+      </c>
+      <c r="C49" t="str">
+        <v>11977665544</v>
+      </c>
+      <c r="D49" t="str">
+        <v>77341583624</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>5</v>
+      </c>
+      <c r="J49">
+        <v>6</v>
+      </c>
+      <c r="K49">
+        <v>7</v>
+      </c>
+      <c r="L49">
+        <v>8</v>
+      </c>
+      <c r="M49">
+        <v>9</v>
+      </c>
+      <c r="N49">
+        <v>10</v>
+      </c>
+      <c r="O49" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B50">
+        <v>1578424633</v>
+      </c>
+      <c r="C50" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D50" t="str">
+        <v>77342981440</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50">
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <v>5</v>
+      </c>
+      <c r="J50">
+        <v>6</v>
+      </c>
+      <c r="K50">
+        <v>7</v>
+      </c>
+      <c r="L50">
+        <v>8</v>
+      </c>
+      <c r="M50">
+        <v>9</v>
+      </c>
+      <c r="N50">
+        <v>10</v>
+      </c>
+      <c r="O50" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B51">
+        <v>1578424633</v>
+      </c>
+      <c r="C51" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D51" t="str">
         <v/>
       </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46">
-        <v>2</v>
-      </c>
-      <c r="G46">
-        <v>3</v>
-      </c>
-      <c r="H46">
-        <v>4</v>
-      </c>
-      <c r="I46">
-        <v>5</v>
-      </c>
-      <c r="J46">
-        <v>6</v>
-      </c>
-      <c r="K46">
-        <v>7</v>
-      </c>
-      <c r="L46">
-        <v>8</v>
-      </c>
-      <c r="M46">
-        <v>9</v>
-      </c>
-      <c r="N46">
-        <v>10</v>
-      </c>
-      <c r="O46" t="str">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+      <c r="H51">
+        <v>4</v>
+      </c>
+      <c r="I51">
+        <v>5</v>
+      </c>
+      <c r="J51">
+        <v>6</v>
+      </c>
+      <c r="K51">
+        <v>7</v>
+      </c>
+      <c r="L51">
+        <v>8</v>
+      </c>
+      <c r="M51">
+        <v>9</v>
+      </c>
+      <c r="N51">
+        <v>10</v>
+      </c>
+      <c r="O51" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B52">
+        <v>1578424633</v>
+      </c>
+      <c r="C52" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D52" t="str">
+        <v/>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>6</v>
+      </c>
+      <c r="K52">
+        <v>7</v>
+      </c>
+      <c r="L52">
+        <v>8</v>
+      </c>
+      <c r="M52">
+        <v>9</v>
+      </c>
+      <c r="N52">
+        <v>10</v>
+      </c>
+      <c r="O52" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B53">
+        <v>1578424633</v>
+      </c>
+      <c r="C53" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D53" t="str">
+        <v/>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
+      <c r="I53">
+        <v>5</v>
+      </c>
+      <c r="J53">
+        <v>6</v>
+      </c>
+      <c r="K53">
+        <v>7</v>
+      </c>
+      <c r="L53">
+        <v>8</v>
+      </c>
+      <c r="M53">
+        <v>9</v>
+      </c>
+      <c r="N53">
+        <v>10</v>
+      </c>
+      <c r="O53" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B54">
+        <v>1578424633</v>
+      </c>
+      <c r="C54" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D54" t="str">
+        <v/>
+      </c>
+      <c r="E54">
+        <v>11</v>
+      </c>
+      <c r="F54">
+        <v>12</v>
+      </c>
+      <c r="G54">
+        <v>13</v>
+      </c>
+      <c r="H54">
+        <v>14</v>
+      </c>
+      <c r="I54">
+        <v>15</v>
+      </c>
+      <c r="J54">
+        <v>16</v>
+      </c>
+      <c r="K54">
+        <v>17</v>
+      </c>
+      <c r="L54">
+        <v>18</v>
+      </c>
+      <c r="M54">
+        <v>19</v>
+      </c>
+      <c r="N54">
+        <v>20</v>
+      </c>
+      <c r="O54" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B55">
+        <v>1578424633</v>
+      </c>
+      <c r="C55" t="str">
+        <v>119988776655</v>
+      </c>
+      <c r="D55" t="str">
+        <v/>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+      <c r="I55">
+        <v>5</v>
+      </c>
+      <c r="J55">
+        <v>6</v>
+      </c>
+      <c r="K55">
+        <v>7</v>
+      </c>
+      <c r="L55">
+        <v>8</v>
+      </c>
+      <c r="M55">
+        <v>9</v>
+      </c>
+      <c r="N55">
+        <v>10</v>
+      </c>
+      <c r="O55" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B56">
+        <v>1578424633</v>
+      </c>
+      <c r="C56" t="str">
+        <v>11977665544</v>
+      </c>
+      <c r="D56" t="str">
+        <v/>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>4</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <v>6</v>
+      </c>
+      <c r="K56">
+        <v>7</v>
+      </c>
+      <c r="L56">
+        <v>8</v>
+      </c>
+      <c r="M56">
+        <v>9</v>
+      </c>
+      <c r="N56">
+        <v>10</v>
+      </c>
+      <c r="O56" t="str">
         <v>Não</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O56"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Faltando apenas resolver o BUG dos números que ao selecionar ele confunde e seleciona o mesmo para vários usuários
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2951,7 +2951,7 @@
         <v>119988776655</v>
       </c>
       <c r="D55" t="str">
-        <v/>
+        <v>77136751137</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -2998,7 +2998,7 @@
         <v>11977665544</v>
       </c>
       <c r="D56" t="str">
-        <v/>
+        <v>77136970483</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -3045,7 +3045,7 @@
         <v>11988776655</v>
       </c>
       <c r="D57" t="str">
-        <v/>
+        <v>77381441200</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -3092,7 +3092,7 @@
         <v>11988776655</v>
       </c>
       <c r="D58" t="str">
-        <v/>
+        <v>77381528772</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -3222,9 +3222,197 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Isabelly Silva Quintans</v>
+      </c>
+      <c r="B61">
+        <v>7117522682</v>
+      </c>
+      <c r="C61" t="str">
+        <v>11966548087</v>
+      </c>
+      <c r="D61" t="str">
+        <v/>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>4</v>
+      </c>
+      <c r="I61">
+        <v>5</v>
+      </c>
+      <c r="J61">
+        <v>6</v>
+      </c>
+      <c r="K61">
+        <v>7</v>
+      </c>
+      <c r="L61">
+        <v>8</v>
+      </c>
+      <c r="M61">
+        <v>9</v>
+      </c>
+      <c r="N61">
+        <v>10</v>
+      </c>
+      <c r="O61" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B62">
+        <v>1578424633</v>
+      </c>
+      <c r="C62" t="str">
+        <v>11987876543</v>
+      </c>
+      <c r="D62" t="str">
+        <v/>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="H62">
+        <v>4</v>
+      </c>
+      <c r="I62">
+        <v>5</v>
+      </c>
+      <c r="J62">
+        <v>6</v>
+      </c>
+      <c r="K62">
+        <v>7</v>
+      </c>
+      <c r="L62">
+        <v>8</v>
+      </c>
+      <c r="M62">
+        <v>9</v>
+      </c>
+      <c r="N62">
+        <v>10</v>
+      </c>
+      <c r="O62" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B63">
+        <v>1578424633</v>
+      </c>
+      <c r="C63" t="str">
+        <v>11987541236</v>
+      </c>
+      <c r="D63" t="str">
+        <v/>
+      </c>
+      <c r="E63">
+        <v>21</v>
+      </c>
+      <c r="F63">
+        <v>26</v>
+      </c>
+      <c r="G63">
+        <v>27</v>
+      </c>
+      <c r="H63">
+        <v>41</v>
+      </c>
+      <c r="I63">
+        <v>43</v>
+      </c>
+      <c r="J63">
+        <v>45</v>
+      </c>
+      <c r="K63">
+        <v>46</v>
+      </c>
+      <c r="L63">
+        <v>49</v>
+      </c>
+      <c r="M63">
+        <v>51</v>
+      </c>
+      <c r="N63">
+        <v>56</v>
+      </c>
+      <c r="O63" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Isabelly Silva Quintans</v>
+      </c>
+      <c r="B64">
+        <v>7117522682</v>
+      </c>
+      <c r="C64" t="str">
+        <v>11987541236</v>
+      </c>
+      <c r="D64" t="str">
+        <v/>
+      </c>
+      <c r="E64">
+        <v>21</v>
+      </c>
+      <c r="F64">
+        <v>26</v>
+      </c>
+      <c r="G64">
+        <v>27</v>
+      </c>
+      <c r="H64">
+        <v>41</v>
+      </c>
+      <c r="I64">
+        <v>43</v>
+      </c>
+      <c r="J64">
+        <v>45</v>
+      </c>
+      <c r="K64">
+        <v>46</v>
+      </c>
+      <c r="L64">
+        <v>49</v>
+      </c>
+      <c r="M64">
+        <v>51</v>
+      </c>
+      <c r="N64">
+        <v>56</v>
+      </c>
+      <c r="O64" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O60"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O64"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Funcionando OK, pronto para TESTE
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3139,7 +3139,7 @@
         <v>11988776655</v>
       </c>
       <c r="D59" t="str">
-        <v/>
+        <v>77163284579</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -3186,7 +3186,7 @@
         <v/>
       </c>
       <c r="D60" t="str">
-        <v/>
+        <v>77163153601</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -3233,7 +3233,7 @@
         <v>11966548087</v>
       </c>
       <c r="D61" t="str">
-        <v/>
+        <v>77407598218</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -3280,7 +3280,7 @@
         <v>11987876543</v>
       </c>
       <c r="D62" t="str">
-        <v/>
+        <v>77407287636</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -3410,9 +3410,197 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B65">
+        <v>1578424633</v>
+      </c>
+      <c r="C65" t="str">
+        <v>11988775544</v>
+      </c>
+      <c r="D65" t="str">
+        <v/>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="H65">
+        <v>4</v>
+      </c>
+      <c r="I65">
+        <v>5</v>
+      </c>
+      <c r="J65">
+        <v>9</v>
+      </c>
+      <c r="K65">
+        <v>10</v>
+      </c>
+      <c r="L65">
+        <v>22</v>
+      </c>
+      <c r="M65">
+        <v>28</v>
+      </c>
+      <c r="N65">
+        <v>29</v>
+      </c>
+      <c r="O65" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B66">
+        <v>1578424633</v>
+      </c>
+      <c r="C66" t="str">
+        <v>11988774455</v>
+      </c>
+      <c r="D66" t="str">
+        <v/>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66">
+        <v>4</v>
+      </c>
+      <c r="I66">
+        <v>5</v>
+      </c>
+      <c r="J66">
+        <v>9</v>
+      </c>
+      <c r="K66">
+        <v>10</v>
+      </c>
+      <c r="L66">
+        <v>22</v>
+      </c>
+      <c r="M66">
+        <v>28</v>
+      </c>
+      <c r="N66">
+        <v>29</v>
+      </c>
+      <c r="O66" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B67">
+        <v>1578424633</v>
+      </c>
+      <c r="C67" t="str">
+        <v/>
+      </c>
+      <c r="D67" t="str">
+        <v/>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>4</v>
+      </c>
+      <c r="I67">
+        <v>5</v>
+      </c>
+      <c r="J67">
+        <v>9</v>
+      </c>
+      <c r="K67">
+        <v>10</v>
+      </c>
+      <c r="L67">
+        <v>22</v>
+      </c>
+      <c r="M67">
+        <v>28</v>
+      </c>
+      <c r="N67">
+        <v>29</v>
+      </c>
+      <c r="O67" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Isabelly Silva Quintans</v>
+      </c>
+      <c r="B68">
+        <v>7117522682</v>
+      </c>
+      <c r="C68" t="str">
+        <v/>
+      </c>
+      <c r="D68" t="str">
+        <v/>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68">
+        <v>4</v>
+      </c>
+      <c r="G68">
+        <v>5</v>
+      </c>
+      <c r="H68">
+        <v>6</v>
+      </c>
+      <c r="I68">
+        <v>7</v>
+      </c>
+      <c r="J68">
+        <v>8</v>
+      </c>
+      <c r="K68">
+        <v>9</v>
+      </c>
+      <c r="L68">
+        <v>10</v>
+      </c>
+      <c r="M68">
+        <v>28</v>
+      </c>
+      <c r="N68">
+        <v>29</v>
+      </c>
+      <c r="O68" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O64"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O68"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aplicação pronta para TESTE (1/2)
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3327,7 +3327,7 @@
         <v>11987541236</v>
       </c>
       <c r="D63" t="str">
-        <v/>
+        <v>77481297146</v>
       </c>
       <c r="E63">
         <v>21</v>
@@ -3598,9 +3598,56 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B69">
+        <v>1578424633</v>
+      </c>
+      <c r="C69" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D69" t="str">
+        <v/>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="H69">
+        <v>4</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+      <c r="J69">
+        <v>9</v>
+      </c>
+      <c r="K69">
+        <v>10</v>
+      </c>
+      <c r="L69">
+        <v>22</v>
+      </c>
+      <c r="M69">
+        <v>28</v>
+      </c>
+      <c r="N69">
+        <v>29</v>
+      </c>
+      <c r="O69" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O68"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O69"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alteração feita em resultados.js, e validações criadas na seleção dos 10 números
</commit_message>
<xml_diff>
--- a/NumerosSelecionados.xlsx
+++ b/NumerosSelecionados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O69"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3374,7 +3374,7 @@
         <v>11987541236</v>
       </c>
       <c r="D64" t="str">
-        <v/>
+        <v>78153849834</v>
       </c>
       <c r="E64">
         <v>21</v>
@@ -3421,7 +3421,7 @@
         <v>11988775544</v>
       </c>
       <c r="D65" t="str">
-        <v/>
+        <v>77908618867</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -3468,7 +3468,7 @@
         <v>11988774455</v>
       </c>
       <c r="D66" t="str">
-        <v/>
+        <v>78159597854</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -3515,7 +3515,7 @@
         <v/>
       </c>
       <c r="D67" t="str">
-        <v/>
+        <v>77912975219</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -3645,9 +3645,197 @@
         <v>Não</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B70">
+        <v>1578424633</v>
+      </c>
+      <c r="C70" t="str">
+        <v>11988776655</v>
+      </c>
+      <c r="D70" t="str">
+        <v/>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <v>4</v>
+      </c>
+      <c r="I70">
+        <v>5</v>
+      </c>
+      <c r="J70">
+        <v>9</v>
+      </c>
+      <c r="K70">
+        <v>10</v>
+      </c>
+      <c r="L70">
+        <v>22</v>
+      </c>
+      <c r="M70">
+        <v>28</v>
+      </c>
+      <c r="N70">
+        <v>29</v>
+      </c>
+      <c r="O70" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Isabelly Silva Quintans</v>
+      </c>
+      <c r="B71">
+        <v>7117522682</v>
+      </c>
+      <c r="C71" t="str">
+        <v/>
+      </c>
+      <c r="D71" t="str">
+        <v/>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <v>4</v>
+      </c>
+      <c r="G71">
+        <v>5</v>
+      </c>
+      <c r="H71">
+        <v>6</v>
+      </c>
+      <c r="I71">
+        <v>7</v>
+      </c>
+      <c r="J71">
+        <v>8</v>
+      </c>
+      <c r="K71">
+        <v>9</v>
+      </c>
+      <c r="L71">
+        <v>10</v>
+      </c>
+      <c r="M71">
+        <v>28</v>
+      </c>
+      <c r="N71">
+        <v>29</v>
+      </c>
+      <c r="O71" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Isabelly Silva Quintans</v>
+      </c>
+      <c r="B72">
+        <v>7117522682</v>
+      </c>
+      <c r="C72" t="str">
+        <v/>
+      </c>
+      <c r="D72" t="str">
+        <v/>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72">
+        <v>4</v>
+      </c>
+      <c r="G72">
+        <v>5</v>
+      </c>
+      <c r="H72">
+        <v>6</v>
+      </c>
+      <c r="I72">
+        <v>7</v>
+      </c>
+      <c r="J72">
+        <v>8</v>
+      </c>
+      <c r="K72">
+        <v>9</v>
+      </c>
+      <c r="L72">
+        <v>10</v>
+      </c>
+      <c r="M72">
+        <v>28</v>
+      </c>
+      <c r="N72">
+        <v>29</v>
+      </c>
+      <c r="O72" t="str">
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Vitor Ito</v>
+      </c>
+      <c r="B73">
+        <v>1578424633</v>
+      </c>
+      <c r="C73" t="str">
+        <v/>
+      </c>
+      <c r="D73" t="str">
+        <v/>
+      </c>
+      <c r="E73">
+        <v>48</v>
+      </c>
+      <c r="F73">
+        <v>51</v>
+      </c>
+      <c r="G73">
+        <v>52</v>
+      </c>
+      <c r="H73">
+        <v>53</v>
+      </c>
+      <c r="I73">
+        <v>54</v>
+      </c>
+      <c r="J73">
+        <v>55</v>
+      </c>
+      <c r="K73">
+        <v>56</v>
+      </c>
+      <c r="L73">
+        <v>57</v>
+      </c>
+      <c r="M73">
+        <v>58</v>
+      </c>
+      <c r="N73">
+        <v>59</v>
+      </c>
+      <c r="O73" t="str">
+        <v>Não</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O69"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O73"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>